<commit_message>
Add COMET score tab to Excel report
</commit_message>
<xml_diff>
--- a/output/reports/translation_report.xlsx
+++ b/output/reports/translation_report.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="composite_score" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bertscore_f1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bleu" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="chrf" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="labse_similarity" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model Rankings" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Language Rankings" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top Combinations" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="comet_score" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bertscore_f1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bleu" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="chrf" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="labse_similarity" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model Rankings" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Language Rankings" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top Combinations" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -498,6 +499,282 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>combination</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>avg_score</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>claude-opus-4.5|spanish</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>claude-opus-4.5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>spanish</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9188465833533653</v>
+      </c>
+      <c r="E2" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>claude-opus-4.5|tagalog</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>claude-opus-4.5</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>tagalog</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.9067619808879903</v>
+      </c>
+      <c r="E3" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>claude-opus-4.5|haitian_creole</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>claude-opus-4.5</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>haitian_creole</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.9061270470103485</v>
+      </c>
+      <c r="E4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>gemini-3-pro|spanish</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>gemini-3-pro</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>spanish</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.8943121417550876</v>
+      </c>
+      <c r="E5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>gpt-5.1|haitian_creole</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>gpt-5.1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>haitian_creole</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.8923091566336027</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>gpt-5.1|spanish</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>gpt-5.1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>spanish</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.8903995964080814</v>
+      </c>
+      <c r="E7" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>claude-opus-4.5|arabic</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>claude-opus-4.5</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>arabic</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.8889351493318415</v>
+      </c>
+      <c r="E8" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>gpt-5.1|tagalog</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>gpt-5.1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>tagalog</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.8880526348141298</v>
+      </c>
+      <c r="E9" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>kimi-k2|spanish</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>kimi-k2</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>spanish</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.8787685138532608</v>
+      </c>
+      <c r="E10" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>claude-opus-4.5|vietnamese</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>claude-opus-4.5</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>vietnamese</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.8779841227374868</v>
+      </c>
+      <c r="E11" t="n">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -746,28 +1023,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9711883415778478</v>
+        <v>0.9107455064853033</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9643870989481608</v>
+        <v>0.9086133142312368</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9794587989648184</v>
+        <v>0.9111654659112295</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9632696857055029</v>
+        <v>0.90642083187898</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9653218388557434</v>
+        <v>0.9081218242645264</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9851500590642294</v>
+        <v>0.9156241019566854</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9794907619555792</v>
+        <v>0.9132047444581985</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9742334634065628</v>
+        <v>0.9107471654812495</v>
       </c>
     </row>
     <row r="3">
@@ -777,28 +1054,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9392301191886266</v>
+        <v>0.896774227420489</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9320045610268911</v>
+        <v>0.8985321124394735</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9373085995515188</v>
+        <v>0.8927175501982371</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9342574526866277</v>
+        <v>0.891526406009992</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9368975212176641</v>
+        <v>0.8960749258597692</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9581400603055954</v>
+        <v>0.9106310854355494</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9504730850458145</v>
+        <v>0.8972395757834116</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9422678997119268</v>
+        <v>0.8977503925561905</v>
       </c>
     </row>
     <row r="4">
@@ -808,28 +1085,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.950635145107905</v>
+        <v>0.8983265161514282</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9405869295199712</v>
+        <v>0.9020032833019892</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9554182837406794</v>
+        <v>0.9060116608937582</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9330211232105891</v>
+        <v>0.8954385370016098</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9522160838047663</v>
+        <v>0.9036827882130941</v>
       </c>
       <c r="G4" t="n">
-        <v>0.961356520652771</v>
+        <v>0.8994199832280477</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9560355742772421</v>
+        <v>0.9104017019271851</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9556755324204763</v>
+        <v>0.9089181621869405</v>
       </c>
     </row>
     <row r="5">
@@ -839,28 +1116,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.953428253531456</v>
+        <v>0.8885662903388342</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9511291037003199</v>
+        <v>0.8956655164559683</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9439690460761389</v>
+        <v>0.853369931379954</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9410848865906397</v>
+        <v>0.881712332367897</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9426348606745402</v>
+        <v>0.8639207283655802</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9616110970576605</v>
+        <v>0.8981739282608032</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9556428541739782</v>
+        <v>0.8935400992631912</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9525100936492285</v>
+        <v>0.8768882602453232</v>
       </c>
     </row>
   </sheetData>
@@ -931,28 +1208,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>65.21080333629443</v>
+        <v>0.9711883415778478</v>
       </c>
       <c r="C2" t="n">
-        <v>52.96399532729856</v>
+        <v>0.9643870989481608</v>
       </c>
       <c r="D2" t="n">
-        <v>71.58286836592715</v>
+        <v>0.9794587989648184</v>
       </c>
       <c r="E2" t="n">
-        <v>51.60042418745073</v>
+        <v>0.9632696857055029</v>
       </c>
       <c r="F2" t="n">
-        <v>54.41753174853448</v>
+        <v>0.9653218388557434</v>
       </c>
       <c r="G2" t="n">
-        <v>76.73282267771704</v>
+        <v>0.9851500590642294</v>
       </c>
       <c r="H2" t="n">
-        <v>73.5266977353005</v>
+        <v>0.9794907619555792</v>
       </c>
       <c r="I2" t="n">
-        <v>61.49267171924929</v>
+        <v>0.9742334634065628</v>
       </c>
     </row>
     <row r="3">
@@ -962,28 +1239,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>55.89622938179431</v>
+        <v>0.9392301191886266</v>
       </c>
       <c r="C3" t="n">
-        <v>43.98356388811123</v>
+        <v>0.9320045610268911</v>
       </c>
       <c r="D3" t="n">
-        <v>51.97885657286032</v>
+        <v>0.9373085995515188</v>
       </c>
       <c r="E3" t="n">
-        <v>38.80762327265631</v>
+        <v>0.9342574526866277</v>
       </c>
       <c r="F3" t="n">
-        <v>43.07356352886825</v>
+        <v>0.9368975212176641</v>
       </c>
       <c r="G3" t="n">
-        <v>68.35135671040831</v>
+        <v>0.9581400603055954</v>
       </c>
       <c r="H3" t="n">
-        <v>63.56959987088033</v>
+        <v>0.9504730850458145</v>
       </c>
       <c r="I3" t="n">
-        <v>50.33510398905668</v>
+        <v>0.9422678997119268</v>
       </c>
     </row>
     <row r="4">
@@ -993,28 +1270,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>60.99839985865118</v>
+        <v>0.950635145107905</v>
       </c>
       <c r="C4" t="n">
-        <v>49.18306122992446</v>
+        <v>0.9405869295199712</v>
       </c>
       <c r="D4" t="n">
-        <v>66.83277953698551</v>
+        <v>0.9554182837406794</v>
       </c>
       <c r="E4" t="n">
-        <v>44.54907968829085</v>
+        <v>0.9330211232105891</v>
       </c>
       <c r="F4" t="n">
-        <v>53.123800801971</v>
+        <v>0.9522160838047663</v>
       </c>
       <c r="G4" t="n">
-        <v>69.09189670541927</v>
+        <v>0.961356520652771</v>
       </c>
       <c r="H4" t="n">
-        <v>68.00742610830768</v>
+        <v>0.9560355742772421</v>
       </c>
       <c r="I4" t="n">
-        <v>60.71471880841934</v>
+        <v>0.9556755324204763</v>
       </c>
     </row>
     <row r="5">
@@ -1024,28 +1301,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>53.3891111383469</v>
+        <v>0.953428253531456</v>
       </c>
       <c r="C5" t="n">
-        <v>44.7683824086141</v>
+        <v>0.9511291037003199</v>
       </c>
       <c r="D5" t="n">
-        <v>49.55283455775599</v>
+        <v>0.9439690460761389</v>
       </c>
       <c r="E5" t="n">
-        <v>33.37028557768944</v>
+        <v>0.9410848865906397</v>
       </c>
       <c r="F5" t="n">
-        <v>39.78171286694072</v>
+        <v>0.9426348606745402</v>
       </c>
       <c r="G5" t="n">
-        <v>60.83174846778979</v>
+        <v>0.9616110970576605</v>
       </c>
       <c r="H5" t="n">
-        <v>60.99319519541403</v>
+        <v>0.9556428541739782</v>
       </c>
       <c r="I5" t="n">
-        <v>49.14371799600143</v>
+        <v>0.9525100936492285</v>
       </c>
     </row>
   </sheetData>
@@ -1116,28 +1393,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>82.27312888275364</v>
+        <v>65.21080333629443</v>
       </c>
       <c r="C2" t="n">
-        <v>76.21131966505428</v>
+        <v>52.96399532729856</v>
       </c>
       <c r="D2" t="n">
-        <v>85.23320310619316</v>
+        <v>71.58286836592715</v>
       </c>
       <c r="E2" t="n">
-        <v>75.51059447715065</v>
+        <v>51.60042418745073</v>
       </c>
       <c r="F2" t="n">
-        <v>75.3871168267268</v>
+        <v>54.41753174853448</v>
       </c>
       <c r="G2" t="n">
-        <v>88.06270663318332</v>
+        <v>76.73282267771704</v>
       </c>
       <c r="H2" t="n">
-        <v>86.63290554048639</v>
+        <v>73.5266977353005</v>
       </c>
       <c r="I2" t="n">
-        <v>79.32847466944554</v>
+        <v>61.49267171924929</v>
       </c>
     </row>
     <row r="3">
@@ -1147,28 +1424,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>79.04481839243751</v>
+        <v>55.89622938179431</v>
       </c>
       <c r="C3" t="n">
-        <v>72.59636517666401</v>
+        <v>43.98356388811123</v>
       </c>
       <c r="D3" t="n">
-        <v>76.67893135331647</v>
+        <v>51.97885657286032</v>
       </c>
       <c r="E3" t="n">
-        <v>68.48648853389588</v>
+        <v>38.80762327265631</v>
       </c>
       <c r="F3" t="n">
-        <v>69.64243838082956</v>
+        <v>43.07356352886825</v>
       </c>
       <c r="G3" t="n">
-        <v>85.61768938663882</v>
+        <v>68.35135671040831</v>
       </c>
       <c r="H3" t="n">
-        <v>83.12568900894648</v>
+        <v>63.56959987088033</v>
       </c>
       <c r="I3" t="n">
-        <v>73.77235655434374</v>
+        <v>50.33510398905668</v>
       </c>
     </row>
     <row r="4">
@@ -1178,28 +1455,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>81.50820324534848</v>
+        <v>60.99839985865118</v>
       </c>
       <c r="C4" t="n">
-        <v>75.48371732005265</v>
+        <v>49.18306122992446</v>
       </c>
       <c r="D4" t="n">
-        <v>84.74052507800789</v>
+        <v>66.83277953698551</v>
       </c>
       <c r="E4" t="n">
-        <v>73.76402818372375</v>
+        <v>44.54907968829085</v>
       </c>
       <c r="F4" t="n">
-        <v>74.91494932667032</v>
+        <v>53.123800801971</v>
       </c>
       <c r="G4" t="n">
-        <v>81.65964406230846</v>
+        <v>69.09189670541927</v>
       </c>
       <c r="H4" t="n">
-        <v>84.53822849416696</v>
+        <v>68.00742610830768</v>
       </c>
       <c r="I4" t="n">
-        <v>80.17125777654867</v>
+        <v>60.71471880841934</v>
       </c>
     </row>
     <row r="5">
@@ -1209,28 +1486,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>76.9219290875521</v>
+        <v>53.3891111383469</v>
       </c>
       <c r="C5" t="n">
-        <v>71.28032192749842</v>
+        <v>44.7683824086141</v>
       </c>
       <c r="D5" t="n">
-        <v>74.7812531322562</v>
+        <v>49.55283455775599</v>
       </c>
       <c r="E5" t="n">
-        <v>63.61623053049644</v>
+        <v>33.37028557768944</v>
       </c>
       <c r="F5" t="n">
-        <v>67.28016338682107</v>
+        <v>39.78171286694072</v>
       </c>
       <c r="G5" t="n">
-        <v>80.51105388853436</v>
+        <v>60.83174846778979</v>
       </c>
       <c r="H5" t="n">
-        <v>81.12855253322255</v>
+        <v>60.99319519541403</v>
       </c>
       <c r="I5" t="n">
-        <v>72.89119430232329</v>
+        <v>49.14371799600143</v>
       </c>
     </row>
   </sheetData>
@@ -1301,28 +1578,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9063588678836823</v>
+        <v>82.27312888275364</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8850996643304825</v>
+        <v>76.21131966505428</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9253268390893936</v>
+        <v>85.23320310619316</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8931691149870554</v>
+        <v>75.51059447715065</v>
       </c>
       <c r="F2" t="n">
-        <v>0.881626029809316</v>
+        <v>75.3871168267268</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9278432875871658</v>
+        <v>88.06270663318332</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9056875507036845</v>
+        <v>86.63290554048639</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8877095431089401</v>
+        <v>79.32847466944554</v>
       </c>
     </row>
     <row r="3">
@@ -1332,28 +1609,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.899536649386088</v>
+        <v>79.04481839243751</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8683734883864721</v>
+        <v>72.59636517666401</v>
       </c>
       <c r="D3" t="n">
-        <v>0.904074082771937</v>
+        <v>76.67893135331647</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8724618405103683</v>
+        <v>68.48648853389588</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8605848997831345</v>
+        <v>69.64243838082956</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9121723075707754</v>
+        <v>85.61768938663882</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8813991993665695</v>
+        <v>83.12568900894648</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8727698028087616</v>
+        <v>73.77235655434374</v>
       </c>
     </row>
     <row r="4">
@@ -1363,28 +1640,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9090816080570221</v>
+        <v>81.50820324534848</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8899000038703283</v>
+        <v>75.48371732005265</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9261859456698099</v>
+        <v>84.74052507800789</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8836089968681335</v>
+        <v>73.76402818372375</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8830699374278387</v>
+        <v>74.91494932667032</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9277814080317816</v>
+        <v>81.65964406230846</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8941338409980139</v>
+        <v>84.53822849416696</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8870414942502975</v>
+        <v>80.17125777654867</v>
       </c>
     </row>
     <row r="5">
@@ -1394,28 +1671,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9090872804323832</v>
+        <v>76.9219290875521</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8846701085567474</v>
+        <v>71.28032192749842</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9185599237680435</v>
+        <v>74.7812531322562</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8805153965950012</v>
+        <v>63.61623053049644</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8710981955130895</v>
+        <v>67.28016338682107</v>
       </c>
       <c r="G5" t="n">
-        <v>0.920716866850853</v>
+        <v>80.51105388853436</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8792760322491328</v>
+        <v>81.12855253322255</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8812564760446548</v>
+        <v>72.89119430232329</v>
       </c>
     </row>
   </sheetData>
@@ -1424,6 +1701,191 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Arabic</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Chinese (Simplified)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Haitian Creole</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Korean</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Russian</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Tagalog/Filipino</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Vietnamese</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>claude-opus-4.5</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.9063588678836823</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.8850996643304825</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9253268390893936</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8931691149870554</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.881626029809316</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9278432875871658</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.9056875507036845</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8877095431089401</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>gemini-3-pro</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.899536649386088</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.8683734883864721</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.904074082771937</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.8724618405103683</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8605848997831345</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9121723075707754</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8813991993665695</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.8727698028087616</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>gpt-5.1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.9090816080570221</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8899000038703283</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.9261859456698099</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.8836089968681335</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8830699374278387</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9277814080317816</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.8941338409980139</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.8870414942502975</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>kimi-k2</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.9090872804323832</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.8846701085567474</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.9185599237680435</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.8805153965950012</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.8710981955130895</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.920716866850853</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.8792760322491328</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.8812564760446548</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1511,7 +1973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1694,280 +2156,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>combination</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>model</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>language</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>avg_score</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>claude-opus-4.5|spanish</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>claude-opus-4.5</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>spanish</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0.9188465833533653</v>
-      </c>
-      <c r="E2" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>claude-opus-4.5|tagalog</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>claude-opus-4.5</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>tagalog</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0.9067619808879903</v>
-      </c>
-      <c r="E3" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>claude-opus-4.5|haitian_creole</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>claude-opus-4.5</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>haitian_creole</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0.9061270470103485</v>
-      </c>
-      <c r="E4" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>gemini-3-pro|spanish</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>gemini-3-pro</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>spanish</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0.8943121417550876</v>
-      </c>
-      <c r="E5" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>gpt-5.1|haitian_creole</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>gpt-5.1</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>haitian_creole</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0.8923091566336027</v>
-      </c>
-      <c r="E6" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>gpt-5.1|spanish</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>gpt-5.1</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>spanish</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>0.8903995964080814</v>
-      </c>
-      <c r="E7" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>claude-opus-4.5|arabic</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>claude-opus-4.5</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>arabic</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>0.8889351493318415</v>
-      </c>
-      <c r="E8" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>gpt-5.1|tagalog</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>gpt-5.1</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>tagalog</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>0.8880526348141298</v>
-      </c>
-      <c r="E9" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>kimi-k2|spanish</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>kimi-k2</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>spanish</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>0.8787685138532608</v>
-      </c>
-      <c r="E10" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>claude-opus-4.5|vietnamese</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>claude-opus-4.5</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>vietnamese</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>0.8779841227374868</v>
-      </c>
-      <c r="E11" t="n">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>